<commit_message>
Added System Requirements and EPS Design Requirements
</commit_message>
<xml_diff>
--- a/CougSat1/CougSat1-Requirements.xlsx
+++ b/CougSat1/CougSat1-Requirements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bradley\Documents\CougsInSpace\CougSat1-Hardware\CougSat1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAB1A648-63C3-4DB3-943E-32E2869C8A8A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61538CBE-9B09-411D-8157-01802A7AAA75}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="726" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="756" uniqueCount="318">
   <si>
     <t>CougSat-1 System Requirements</t>
   </si>
@@ -605,24 +605,6 @@
     <t>Need to process mission critical events as they happen.</t>
   </si>
   <si>
-    <t>Must comply with CubeSat Specifications Rev 13 section 2: P-Pod Interface</t>
-  </si>
-  <si>
-    <t>Must comply with CubeSat Specifications Rev 13 section 3.1: General</t>
-  </si>
-  <si>
-    <t>Must comply with CubeSat Specifications Rev 13 section 3.2: Mechanical</t>
-  </si>
-  <si>
-    <t>Must comply with CubeSat Specifications Rev 13 section 3.3: Electrical</t>
-  </si>
-  <si>
-    <t>Must comply with CubeSat Specifications Rev 13 section 3.4: Operational</t>
-  </si>
-  <si>
-    <t>Must comply with CubeSat Specifications Rev 13 section 4: Testing</t>
-  </si>
-  <si>
     <t>CougSat-1 shall adhere to all requirements for the NASA CubeSat Launch Initiative</t>
   </si>
   <si>
@@ -704,169 +686,301 @@
     <t>EPS-022</t>
   </si>
   <si>
-    <t>EPS-023</t>
-  </si>
-  <si>
-    <t>EPS-024</t>
-  </si>
-  <si>
-    <t>EPS-025</t>
-  </si>
-  <si>
-    <t>EPS-026</t>
-  </si>
-  <si>
-    <t>EPS-027</t>
-  </si>
-  <si>
-    <t>EPS-028</t>
-  </si>
-  <si>
-    <t>EPS-029</t>
-  </si>
-  <si>
-    <t>EPS-030</t>
-  </si>
-  <si>
-    <t>EPS-031</t>
-  </si>
-  <si>
-    <t>EPS-032</t>
-  </si>
-  <si>
-    <t>EPS-033</t>
-  </si>
-  <si>
-    <t>EPS-034</t>
-  </si>
-  <si>
-    <t>EPS-035</t>
-  </si>
-  <si>
-    <t>EPS-036</t>
-  </si>
-  <si>
-    <t>EPS-037</t>
-  </si>
-  <si>
-    <t>EPS-038</t>
-  </si>
-  <si>
-    <t>EPS-039</t>
-  </si>
-  <si>
-    <t>EPS-040</t>
-  </si>
-  <si>
-    <t>EPS-041</t>
-  </si>
-  <si>
-    <t>EPS-042</t>
-  </si>
-  <si>
-    <t>EPS-043</t>
-  </si>
-  <si>
-    <t>EPS-044</t>
-  </si>
-  <si>
-    <t>EPS-045</t>
-  </si>
-  <si>
-    <t>EPS-046</t>
-  </si>
-  <si>
-    <t>EPS-047</t>
-  </si>
-  <si>
-    <t>EPS-048</t>
-  </si>
-  <si>
-    <t>EPS-049</t>
-  </si>
-  <si>
-    <t>EPS-050</t>
-  </si>
-  <si>
-    <t>EPS-051</t>
-  </si>
-  <si>
-    <t>EPS-052</t>
-  </si>
-  <si>
-    <t>EPS-053</t>
-  </si>
-  <si>
-    <t>EPS-054</t>
-  </si>
-  <si>
-    <t>EPS-055</t>
-  </si>
-  <si>
-    <t>EPS-056</t>
-  </si>
-  <si>
-    <t>EPS-057</t>
-  </si>
-  <si>
-    <t>EPS-058</t>
-  </si>
-  <si>
-    <t>EPS-059</t>
-  </si>
-  <si>
-    <t>EPS-060</t>
-  </si>
-  <si>
-    <t>EPS-061</t>
-  </si>
-  <si>
-    <t>EPS-062</t>
-  </si>
-  <si>
-    <t>EPS-063</t>
-  </si>
-  <si>
-    <t>EPS-064</t>
-  </si>
-  <si>
-    <t>EPS-065</t>
-  </si>
-  <si>
-    <t>EPS-066</t>
-  </si>
-  <si>
-    <t>EPS-067</t>
-  </si>
-  <si>
-    <t>EPS-068</t>
-  </si>
-  <si>
-    <t>EPS-069</t>
-  </si>
-  <si>
-    <t>EPS-070</t>
-  </si>
-  <si>
-    <t>EPS-071</t>
-  </si>
-  <si>
-    <t>EPS-072</t>
-  </si>
-  <si>
-    <t>EPS-073</t>
-  </si>
-  <si>
-    <t>EPS-074</t>
-  </si>
-  <si>
-    <t>EPS-075</t>
-  </si>
-  <si>
-    <t>EPS-076</t>
-  </si>
-  <si>
-    <t>Derrieved From System Requirement(s)</t>
+    <t>REQ-000</t>
+  </si>
+  <si>
+    <t>CougSat-1 and CougsInSpace's ground station shall comply with all requirements listed below</t>
+  </si>
+  <si>
+    <t>Requirements are required</t>
+  </si>
+  <si>
+    <t>CougSat-1 shall comply with CubeSat Specifications Rev 13 section 2: P-Pod Interface</t>
+  </si>
+  <si>
+    <t>CougSat-1 shall comply with CubeSat Specifications Rev 13 section 3.1: General</t>
+  </si>
+  <si>
+    <t>CougSat-1 shall comply with CubeSat Specifications Rev 13 section 3.2: Mechanical</t>
+  </si>
+  <si>
+    <t>CougSat-1 shall comply with CubeSat Specifications Rev 13 section 3.3: Electrical</t>
+  </si>
+  <si>
+    <t>CougSat-1 shall comply with CubeSat Specifications Rev 13 section 3.4: Operational</t>
+  </si>
+  <si>
+    <t>CougSat-1 shall comply with CubeSat Specifications Rev 13 section 4: Testing</t>
+  </si>
+  <si>
+    <t>CougSat-1's bus shall be reused on future CougSats</t>
+  </si>
+  <si>
+    <t>Mission Objective 1</t>
+  </si>
+  <si>
+    <t>Desired</t>
+  </si>
+  <si>
+    <t>CougSat-1 shall have a reliable and robust bus</t>
+  </si>
+  <si>
+    <t>CougSat-1 may have a plant germination experiment payload for up to 30 days</t>
+  </si>
+  <si>
+    <t>Mission Objective 2</t>
+  </si>
+  <si>
+    <t>CougSat-1 shall transfer, to ground, all data from all payloads</t>
+  </si>
+  <si>
+    <t>Payloads need to be analyzed on the ground</t>
+  </si>
+  <si>
+    <t>CougSat-1 shall have at least one WSU Cougar logo</t>
+  </si>
+  <si>
+    <t>Mission Objective 3 &amp; Go Cougs!</t>
+  </si>
+  <si>
+    <t>CougSat-1 may transmit "Go Cougs!" over voice around the world</t>
+  </si>
+  <si>
+    <t>Cosmetic</t>
+  </si>
+  <si>
+    <t>Only a single ground station is planned in Pullman</t>
+  </si>
+  <si>
+    <t>CougSat-1 shall operate without contact from the ground for up to 10 days</t>
+  </si>
+  <si>
+    <t>CougSat-1 shall communicate at least with a CougsInSpace's ground station</t>
+  </si>
+  <si>
+    <t>CougSat-1 may reprogram any of its programmable processors</t>
+  </si>
+  <si>
+    <t>Mission Objective 4</t>
+  </si>
+  <si>
+    <t>CougsInSpace's ground station may be developed and operated by individuals or groups outside of CougsInSpace</t>
+  </si>
+  <si>
+    <t>Must be easily reproduced and used</t>
+  </si>
+  <si>
+    <t>Only CougsInSpace's ground stations operated by CougsInSpace shall have transmit capabilities</t>
+  </si>
+  <si>
+    <t>Security</t>
+  </si>
+  <si>
+    <t>CougSat-1 shall transfer, to ground, telemetry</t>
+  </si>
+  <si>
+    <t>All components fail when exposed to extreme temperatures</t>
+  </si>
+  <si>
+    <t>CougSat-1 shall slew</t>
+  </si>
+  <si>
+    <t>Need to change attitude for payload and health reasons</t>
+  </si>
+  <si>
+    <t>CougSat-1 shall have at least one electrical subsystem powered beginning after ejection from the P-Pod for the mission duration</t>
+  </si>
+  <si>
+    <t>CougSat-1 shall be single fault tolerant</t>
+  </si>
+  <si>
+    <t>CougSat-1 should be functional for the entire mission duration</t>
+  </si>
+  <si>
+    <t>CougSat-1 will buffer data until successful reception from the ground</t>
+  </si>
+  <si>
+    <t>CougsInSpace shall have a single archive for all data with at least a backup</t>
+  </si>
+  <si>
+    <t>Losing the data negates all progress</t>
+  </si>
+  <si>
+    <t>CougSat-1 shall have testing procedures created</t>
+  </si>
+  <si>
+    <t>In order to validate REQ-009</t>
+  </si>
+  <si>
+    <t>CougSat-1 shall pass all CougSat-1 test procedures</t>
+  </si>
+  <si>
+    <t>Photos can help promote the club and its mission</t>
+  </si>
+  <si>
+    <t>The EPS shall have at least two voltage outputs</t>
+  </si>
+  <si>
+    <t>Different components require different voltages</t>
+  </si>
+  <si>
+    <t>Components expect a voltage and should be given that voltage</t>
+  </si>
+  <si>
+    <t>Smooth voltage rails reduces stress on components</t>
+  </si>
+  <si>
+    <t>The EPS shall keep enabled regulated rails' average voltage within 5%</t>
+  </si>
+  <si>
+    <t>The EPS shall keep enabled regulated rails' voltage ripple to less than 0.5%</t>
+  </si>
+  <si>
+    <t>The EPS shall keep enabled regulated rails' voltage noise to less than 1%</t>
+  </si>
+  <si>
+    <t>An energy budget shows an average use of 1.6W</t>
+  </si>
+  <si>
+    <t>The EPS shall be capable of providing 10W of peak power to loads for 10 minutes each orbit</t>
+  </si>
+  <si>
+    <t>An energy budget shows an peak use of 8.5W</t>
+  </si>
+  <si>
+    <t>The EPS shall be capable of providing 2W continuously to loads including during periods of eclipse from the earth</t>
+  </si>
+  <si>
+    <t>Wasted power is unusable and undesirably raises the temperature of the satellite</t>
+  </si>
+  <si>
+    <t>REQ-009, REQ-025</t>
+  </si>
+  <si>
+    <t>The EPS shall have energy storage devices</t>
+  </si>
+  <si>
+    <t>Need to operate while in the shade (eclipsed by the earth)</t>
+  </si>
+  <si>
+    <t>REQ-009, REQ-024</t>
+  </si>
+  <si>
+    <t>The EPS shall use photovoltaics to capture energy from the sun</t>
+  </si>
+  <si>
+    <t>The sun outputs a lot of easily obtained and reliable power</t>
+  </si>
+  <si>
+    <t>The EPS shall monitor the current consumption of each load</t>
+  </si>
+  <si>
+    <t>Overcurrent consumption needs to be halted</t>
+  </si>
+  <si>
+    <t>The EPS shall be capable of disabling each load</t>
+  </si>
+  <si>
+    <t>Low power states needs to controlled</t>
+  </si>
+  <si>
+    <t>If the PMIC turns off, it may not be able to turn back on</t>
+  </si>
+  <si>
+    <t>REQ-009, REQ-024, REQ-0025</t>
+  </si>
+  <si>
+    <t>When the stored energy is nearing being exhausted, it needs to be prioritized for preserving the health of the satellite</t>
+  </si>
+  <si>
+    <t>REQ-009, REQ-024, REQ-025</t>
+  </si>
+  <si>
+    <t>The EPS shall monitor the power production from each solar cell</t>
+  </si>
+  <si>
+    <t>The EPS shall monitor the energy level in its energy storage devices</t>
+  </si>
+  <si>
+    <t>The EPS shall monitor the temperature of each component in the power chain</t>
+  </si>
+  <si>
+    <t>REQ-009, REQ-021</t>
+  </si>
+  <si>
+    <t>Power level can be used to aid the ADCS in aiming the solar cells</t>
+  </si>
+  <si>
+    <t>The EPS needs to know when to enter safe mode</t>
+  </si>
+  <si>
+    <t>The EPS shall communicate to the IHU</t>
+  </si>
+  <si>
+    <t>The EPS needs to receive commands from the IHU and alert it when entering safe mode</t>
+  </si>
+  <si>
+    <t>The EPS shall send telemetry to the IHU upon request</t>
+  </si>
+  <si>
+    <t>The IHU logs the data and sends it to the ground for analysis</t>
+  </si>
+  <si>
+    <t>The EPS shall have a RBF pin and deployment switches that disconnect all loads from the power chain</t>
+  </si>
+  <si>
+    <t>When in the P-POD, the entire satellite needs to be off</t>
+  </si>
+  <si>
+    <t>The EPS shall be capable of using power from the umbilical during testing</t>
+  </si>
+  <si>
+    <t>The EPS shall have a single PMIC whose role is to monitor the EPS, control the EPS, and communicate with the IHU</t>
+  </si>
+  <si>
+    <t>More than one processor increase complexity and may reduce reliability at the cost of increased redundancy</t>
+  </si>
+  <si>
+    <t>Derived From System Requirement(s)</t>
+  </si>
+  <si>
+    <t>The EPS shall have an efficiency of at least 90% during average continuous load</t>
+  </si>
+  <si>
+    <t>The EPS shall have two independent power chains with capabilities to route inputs and/or outputs to either chain</t>
+  </si>
+  <si>
+    <t>Independent power chains increases redundancy. Routing inputs/outputs allow load balancing and avoiding faulty components</t>
+  </si>
+  <si>
+    <t>The EPS shall have an regulated rail for the PMIC that is always on between the ejection from the P-POD for the mission duration</t>
+  </si>
+  <si>
+    <t>The EPS shall be capable of entering safe mode where only critical subsystems are enabled</t>
+  </si>
+  <si>
+    <t>The EPS needs to know when to enter safe mode. The ADCS needs to know when to aid in temperature regulation</t>
+  </si>
+  <si>
+    <t>Need to operate the entire satellite without requiring an artificial Sun</t>
+  </si>
+  <si>
+    <t>We don't want to transmit all data every time, and we don't want to lose data</t>
+  </si>
+  <si>
+    <t>CougSat-1 may have a camera capable of photographing the earth in the visible spectrum</t>
+  </si>
+  <si>
+    <t>CougSat-1 may not have continuous contact with the ground</t>
+  </si>
+  <si>
+    <t>CougsInSpace's remote ground stations may send all received data to CougsInSpace</t>
+  </si>
+  <si>
+    <t>A single repository shall hold all data from CougSat-1</t>
+  </si>
+  <si>
+    <t>CougSat-1 shall keep all components within prescribed operational temperature ranges beginning after ejection from the P-Pod for the mission duration</t>
   </si>
 </sst>
 </file>
@@ -918,7 +1032,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -934,6 +1048,24 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1252,40 +1384,41 @@
   <dimension ref="A1:G79"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <pane ySplit="3" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.140625" customWidth="1"/>
-    <col min="2" max="2" width="72.28515625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="50.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" style="10" customWidth="1"/>
+    <col min="2" max="2" width="78.85546875" style="13" customWidth="1"/>
+    <col min="3" max="3" width="60.5703125" style="13" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:7" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
     </row>
     <row r="3" spans="1:7" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
@@ -1305,673 +1438,889 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="10" t="s">
+        <v>219</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>221</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>194</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>199</v>
-      </c>
-      <c r="D4" t="s">
-        <v>200</v>
-      </c>
-      <c r="E4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="B5" s="13" t="s">
+        <v>192</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>193</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>194</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>192</v>
-      </c>
-      <c r="C5" s="4" t="s">
+      <c r="B6" s="13" t="s">
+        <v>222</v>
+      </c>
+      <c r="C6" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="D5" t="s">
-        <v>200</v>
-      </c>
-      <c r="E5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="D6" s="10" t="s">
+        <v>194</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>193</v>
-      </c>
-      <c r="C6" s="4" t="s">
+      <c r="B7" s="13" t="s">
+        <v>223</v>
+      </c>
+      <c r="C7" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="D6" t="s">
-        <v>200</v>
-      </c>
-      <c r="E6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="D7" s="10" t="s">
+        <v>194</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B8" s="13" t="s">
+        <v>224</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="10" t="s">
         <v>194</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="E8" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>225</v>
+      </c>
+      <c r="C9" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="D7" t="s">
-        <v>200</v>
-      </c>
-      <c r="E7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>195</v>
-      </c>
-      <c r="C8" s="4" t="s">
+      <c r="D9" s="10" t="s">
+        <v>194</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>226</v>
+      </c>
+      <c r="C10" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="D8" t="s">
-        <v>200</v>
-      </c>
-      <c r="E8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="C9" s="4" t="s">
+      <c r="D10" s="10" t="s">
+        <v>194</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>227</v>
+      </c>
+      <c r="C11" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="D9" t="s">
-        <v>200</v>
-      </c>
-      <c r="E9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>197</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" t="s">
-        <v>200</v>
-      </c>
-      <c r="E10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="D11" s="10" t="s">
+        <v>194</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="E11" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+      <c r="B12" s="13" t="s">
+        <v>228</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>229</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>230</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="E12" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+      <c r="B13" s="13" t="s">
+        <v>231</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>229</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>194</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="E13" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+      <c r="B14" s="13" t="s">
+        <v>232</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>233</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>230</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="E14" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+      <c r="B15" s="13" t="s">
+        <v>234</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>235</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>230</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="E15" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+      <c r="B16" s="13" t="s">
+        <v>236</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>237</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>194</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="E16" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+      <c r="B17" s="13" t="s">
+        <v>238</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>182</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>239</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="E17" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+      <c r="B18" s="13" t="s">
+        <v>314</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>240</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>194</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="E18" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
+      <c r="B19" s="13" t="s">
+        <v>241</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>194</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="E19" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
+      <c r="B20" s="13" t="s">
+        <v>242</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>240</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>194</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="E20" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
+      <c r="B21" s="13" t="s">
+        <v>243</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>244</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>230</v>
+      </c>
+      <c r="E21" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="E21" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
+      <c r="B22" s="13" t="s">
+        <v>245</v>
+      </c>
+      <c r="C22" s="13" t="s">
+        <v>246</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>194</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="E22" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
+      <c r="B23" s="13" t="s">
+        <v>315</v>
+      </c>
+      <c r="C23" s="13" t="s">
+        <v>316</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>230</v>
+      </c>
+      <c r="E23" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="E23" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
+      <c r="B24" s="13" t="s">
+        <v>247</v>
+      </c>
+      <c r="C24" s="13" t="s">
+        <v>248</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>194</v>
+      </c>
+      <c r="E24" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="E24" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
+      <c r="B25" s="13" t="s">
+        <v>249</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>229</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>194</v>
+      </c>
+      <c r="E25" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="E25" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
+      <c r="B26" s="13" t="s">
+        <v>317</v>
+      </c>
+      <c r="C26" s="13" t="s">
+        <v>250</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>194</v>
+      </c>
+      <c r="E26" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="E26" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
+      <c r="B27" s="13" t="s">
+        <v>251</v>
+      </c>
+      <c r="C27" s="13" t="s">
+        <v>252</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>194</v>
+      </c>
+      <c r="E27" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="E27" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
+      <c r="B28" s="13" t="s">
+        <v>253</v>
+      </c>
+      <c r="C28" s="13" t="s">
+        <v>159</v>
+      </c>
+      <c r="D28" s="10" t="s">
+        <v>194</v>
+      </c>
+      <c r="E28" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="E28" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
+      <c r="B29" s="13" t="s">
+        <v>254</v>
+      </c>
+      <c r="C29" s="13" t="s">
+        <v>255</v>
+      </c>
+      <c r="D29" s="10" t="s">
+        <v>230</v>
+      </c>
+      <c r="E29" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="E29" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
+      <c r="B30" s="13" t="s">
+        <v>256</v>
+      </c>
+      <c r="C30" s="13" t="s">
+        <v>312</v>
+      </c>
+      <c r="D30" s="10" t="s">
+        <v>194</v>
+      </c>
+      <c r="E30" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="E30" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
+      <c r="B31" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="C31" s="13" t="s">
+        <v>258</v>
+      </c>
+      <c r="D31" s="10" t="s">
+        <v>194</v>
+      </c>
+      <c r="E31" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="E31" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
+      <c r="B32" s="13" t="s">
+        <v>259</v>
+      </c>
+      <c r="C32" s="13" t="s">
+        <v>260</v>
+      </c>
+      <c r="D32" s="10" t="s">
+        <v>194</v>
+      </c>
+      <c r="E32" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="E32" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
+      <c r="B33" s="13" t="s">
+        <v>261</v>
+      </c>
+      <c r="C33" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="D33" s="10" t="s">
+        <v>194</v>
+      </c>
+      <c r="E33" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="E33" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="E34" t="s">
+      <c r="B34" s="13" t="s">
+        <v>313</v>
+      </c>
+      <c r="C34" s="13" t="s">
+        <v>262</v>
+      </c>
+      <c r="D34" s="10" t="s">
+        <v>230</v>
+      </c>
+      <c r="E34" s="10" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
+      <c r="A35" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="E35" t="s">
+      <c r="E35" s="10" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
+      <c r="A36" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="E36" t="s">
+      <c r="E36" s="10" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
+      <c r="A37" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="E37" t="s">
+      <c r="E37" s="10" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
+      <c r="A38" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="E38" t="s">
+      <c r="E38" s="10" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
+      <c r="A39" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="E39" t="s">
+      <c r="E39" s="10" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
+      <c r="A40" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="E40" t="s">
+      <c r="E40" s="10" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="2" t="s">
+      <c r="A41" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="E41" t="s">
+      <c r="E41" s="10" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="2" t="s">
+      <c r="A42" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="E42" t="s">
+      <c r="E42" s="10" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="2" t="s">
+      <c r="A43" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="E43" t="s">
+      <c r="E43" s="10" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="2" t="s">
+      <c r="A44" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="E44" t="s">
+      <c r="E44" s="10" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="2" t="s">
+      <c r="A45" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="E45" t="s">
+      <c r="E45" s="10" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="2" t="s">
+      <c r="A46" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="E46" t="s">
+      <c r="E46" s="10" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="2" t="s">
+      <c r="A47" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="E47" t="s">
+      <c r="E47" s="10" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="2" t="s">
+      <c r="A48" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="E48" t="s">
+      <c r="E48" s="10" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="2" t="s">
+      <c r="A49" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="E49" t="s">
+      <c r="E49" s="10" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="2" t="s">
+      <c r="A50" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="E50" t="s">
+      <c r="E50" s="10" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="2" t="s">
+      <c r="A51" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="E51" t="s">
+      <c r="E51" s="10" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="2" t="s">
+      <c r="A52" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="E52" t="s">
+      <c r="E52" s="10" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="2" t="s">
+      <c r="A53" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="E53" t="s">
+      <c r="E53" s="10" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="2" t="s">
+      <c r="A54" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="E54" t="s">
+      <c r="E54" s="10" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="2" t="s">
+      <c r="A55" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="E55" t="s">
+      <c r="E55" s="10" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="2" t="s">
+      <c r="A56" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="E56" t="s">
+      <c r="E56" s="10" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="2" t="s">
+      <c r="A57" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="E57" t="s">
+      <c r="E57" s="10" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="2" t="s">
+      <c r="A58" s="10" t="s">
         <v>126</v>
       </c>
-      <c r="E58" t="s">
+      <c r="E58" s="10" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" s="2" t="s">
+      <c r="A59" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="E59" t="s">
+      <c r="E59" s="10" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" s="2" t="s">
+      <c r="A60" s="10" t="s">
         <v>128</v>
       </c>
-      <c r="E60" t="s">
+      <c r="E60" s="10" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61" s="2" t="s">
+      <c r="A61" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="E61" t="s">
+      <c r="E61" s="10" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" s="2" t="s">
+      <c r="A62" s="10" t="s">
         <v>130</v>
       </c>
-      <c r="E62" t="s">
+      <c r="E62" s="10" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A63" s="2" t="s">
+      <c r="A63" s="10" t="s">
         <v>131</v>
       </c>
-      <c r="E63" t="s">
+      <c r="E63" s="10" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A64" s="2" t="s">
+      <c r="A64" s="10" t="s">
         <v>132</v>
       </c>
-      <c r="E64" t="s">
+      <c r="E64" s="10" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A65" s="2" t="s">
+      <c r="A65" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="E65" t="s">
+      <c r="E65" s="10" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" s="2" t="s">
+      <c r="A66" s="10" t="s">
         <v>134</v>
       </c>
-      <c r="E66" t="s">
+      <c r="E66" s="10" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67" s="2" t="s">
+      <c r="A67" s="10" t="s">
         <v>135</v>
       </c>
-      <c r="E67" t="s">
+      <c r="E67" s="10" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" s="2" t="s">
+      <c r="A68" s="10" t="s">
         <v>136</v>
       </c>
-      <c r="E68" t="s">
+      <c r="E68" s="10" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A69" s="2" t="s">
+      <c r="A69" s="10" t="s">
         <v>137</v>
       </c>
-      <c r="E69" t="s">
+      <c r="E69" s="10" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70" s="2" t="s">
+      <c r="A70" s="10" t="s">
         <v>138</v>
       </c>
-      <c r="E70" t="s">
+      <c r="E70" s="10" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A71" s="2" t="s">
+      <c r="A71" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="E71" t="s">
+      <c r="E71" s="10" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A72" s="2" t="s">
+      <c r="A72" s="10" t="s">
         <v>140</v>
       </c>
-      <c r="E72" t="s">
+      <c r="E72" s="10" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A73" s="2" t="s">
+      <c r="A73" s="10" t="s">
         <v>141</v>
       </c>
-      <c r="E73" t="s">
+      <c r="E73" s="10" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A74" s="2" t="s">
+      <c r="A74" s="10" t="s">
         <v>142</v>
       </c>
-      <c r="E74" t="s">
+      <c r="E74" s="10" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A75" s="2" t="s">
+      <c r="A75" s="10" t="s">
         <v>144</v>
       </c>
-      <c r="E75" t="s">
+      <c r="E75" s="10" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A76" s="2" t="s">
+      <c r="A76" s="10" t="s">
         <v>145</v>
       </c>
-      <c r="E76" t="s">
+      <c r="E76" s="10" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A77" s="2" t="s">
+      <c r="A77" s="10" t="s">
         <v>184</v>
       </c>
-      <c r="E77" t="s">
+      <c r="E77" s="10" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A78" s="2" t="s">
+      <c r="A78" s="10" t="s">
         <v>188</v>
       </c>
-      <c r="E78" t="s">
+      <c r="E78" s="10" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A79" s="2" t="s">
+      <c r="A79" s="10" t="s">
         <v>189</v>
       </c>
-      <c r="E79" t="s">
+      <c r="E79" s="10" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1987,43 +2336,44 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D8478C5-1713-4B9E-8DAE-5F54C2737D56}">
-  <dimension ref="A1:G79"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
+      <pane ySplit="3" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.140625" customWidth="1"/>
-    <col min="2" max="2" width="72.28515625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="50.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.28515625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" style="10" customWidth="1"/>
+    <col min="2" max="2" width="72.28515625" style="13" customWidth="1"/>
+    <col min="3" max="3" width="59.140625" style="13" customWidth="1"/>
+    <col min="4" max="4" width="26.140625" style="13" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="6" t="s">
-        <v>201</v>
-      </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
+    <row r="1" spans="1:7" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
-        <v>202</v>
-      </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
+      <c r="A2" s="11" t="s">
+        <v>196</v>
+      </c>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
     </row>
     <row r="3" spans="1:7" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
@@ -2036,617 +2386,383 @@
         <v>4</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>279</v>
+        <v>304</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>263</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>264</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>198</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>267</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>265</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>269</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>266</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
+        <v>200</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>268</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>266</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
+        <v>201</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>273</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>270</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
+        <v>202</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>271</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>272</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
         <v>203</v>
       </c>
-      <c r="E4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="B10" s="13" t="s">
+        <v>305</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>274</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
         <v>204</v>
       </c>
-      <c r="E5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="B11" s="13" t="s">
+        <v>306</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>307</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>275</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
         <v>205</v>
       </c>
-      <c r="E6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="B12" s="13" t="s">
+        <v>276</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>277</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>278</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
         <v>206</v>
       </c>
-      <c r="E7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="B13" s="13" t="s">
+        <v>279</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>280</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="10" t="s">
         <v>207</v>
       </c>
-      <c r="E8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="B14" s="13" t="s">
+        <v>281</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>282</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="10" t="s">
         <v>208</v>
       </c>
-      <c r="E9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="B15" s="13" t="s">
+        <v>283</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>284</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="10" t="s">
         <v>209</v>
       </c>
-      <c r="E10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="B16" s="13" t="s">
+        <v>308</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>285</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>286</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="10" t="s">
         <v>210</v>
       </c>
-      <c r="E11" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+      <c r="B17" s="13" t="s">
+        <v>309</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>287</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>288</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="10" t="s">
         <v>211</v>
       </c>
-      <c r="E12" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+      <c r="B18" s="13" t="s">
+        <v>289</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>293</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>292</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="10" t="s">
         <v>212</v>
       </c>
-      <c r="E13" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+      <c r="B19" s="13" t="s">
+        <v>290</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>294</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>292</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="10" t="s">
         <v>213</v>
       </c>
-      <c r="E14" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+      <c r="B20" s="13" t="s">
+        <v>291</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>310</v>
+      </c>
+      <c r="D20" s="13" t="s">
+        <v>292</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="10" t="s">
         <v>214</v>
       </c>
-      <c r="E15" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+      <c r="B21" s="13" t="s">
+        <v>295</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>296</v>
+      </c>
+      <c r="D21" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="E21" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="10" t="s">
         <v>215</v>
       </c>
-      <c r="E16" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+      <c r="B22" s="13" t="s">
+        <v>297</v>
+      </c>
+      <c r="C22" s="13" t="s">
+        <v>298</v>
+      </c>
+      <c r="D22" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="10" t="s">
         <v>216</v>
       </c>
-      <c r="E17" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+      <c r="B23" s="13" t="s">
+        <v>299</v>
+      </c>
+      <c r="C23" s="13" t="s">
+        <v>300</v>
+      </c>
+      <c r="D23" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="E23" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="10" t="s">
         <v>217</v>
       </c>
-      <c r="E18" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
+      <c r="B24" s="13" t="s">
+        <v>301</v>
+      </c>
+      <c r="C24" s="13" t="s">
+        <v>311</v>
+      </c>
+      <c r="D24" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="E24" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="10" t="s">
         <v>218</v>
       </c>
-      <c r="E19" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="E20" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="E21" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="E22" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="E23" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="E24" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="E25" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="E26" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="E27" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="E28" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="E29" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="E30" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="E31" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
-        <v>231</v>
-      </c>
-      <c r="E32" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="E33" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="E34" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="E35" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="E36" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="E37" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="E38" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="E39" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
-        <v>239</v>
-      </c>
-      <c r="E40" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="E41" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="E42" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="2" t="s">
-        <v>242</v>
-      </c>
-      <c r="E43" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="E44" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="2" t="s">
-        <v>244</v>
-      </c>
-      <c r="E45" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="E46" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="E47" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="E48" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="E49" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="E50" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="E51" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="E52" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="2" t="s">
-        <v>252</v>
-      </c>
-      <c r="E53" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="2" t="s">
-        <v>253</v>
-      </c>
-      <c r="E54" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="2" t="s">
-        <v>254</v>
-      </c>
-      <c r="E55" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="2" t="s">
-        <v>255</v>
-      </c>
-      <c r="E56" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="2" t="s">
-        <v>256</v>
-      </c>
-      <c r="E57" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="2" t="s">
-        <v>257</v>
-      </c>
-      <c r="E58" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" s="2" t="s">
-        <v>258</v>
-      </c>
-      <c r="E59" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" s="2" t="s">
-        <v>259</v>
-      </c>
-      <c r="E60" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61" s="2" t="s">
-        <v>260</v>
-      </c>
-      <c r="E61" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" s="2" t="s">
-        <v>261</v>
-      </c>
-      <c r="E62" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A63" s="2" t="s">
-        <v>262</v>
-      </c>
-      <c r="E63" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A64" s="2" t="s">
-        <v>263</v>
-      </c>
-      <c r="E64" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A65" s="2" t="s">
-        <v>264</v>
-      </c>
-      <c r="E65" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" s="2" t="s">
-        <v>265</v>
-      </c>
-      <c r="E66" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67" s="2" t="s">
-        <v>266</v>
-      </c>
-      <c r="E67" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" s="2" t="s">
-        <v>267</v>
-      </c>
-      <c r="E68" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A69" s="2" t="s">
-        <v>268</v>
-      </c>
-      <c r="E69" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70" s="2" t="s">
-        <v>269</v>
-      </c>
-      <c r="E70" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A71" s="2" t="s">
-        <v>270</v>
-      </c>
-      <c r="E71" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A72" s="2" t="s">
-        <v>271</v>
-      </c>
-      <c r="E72" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A73" s="2" t="s">
-        <v>272</v>
-      </c>
-      <c r="E73" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A74" s="2" t="s">
-        <v>273</v>
-      </c>
-      <c r="E74" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A75" s="2" t="s">
-        <v>274</v>
-      </c>
-      <c r="E75" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A76" s="2" t="s">
+      <c r="B25" s="13" t="s">
+        <v>302</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>303</v>
+      </c>
+      <c r="D25" s="13" t="s">
         <v>275</v>
       </c>
-      <c r="E76" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A77" s="2" t="s">
-        <v>276</v>
-      </c>
-      <c r="E77" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A78" s="2" t="s">
-        <v>277</v>
-      </c>
-      <c r="E78" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A79" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="E79" t="s">
+      <c r="E25" s="10" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added C&DH, ECS, and Structure Design Requirements
</commit_message>
<xml_diff>
--- a/CougSat1/CougSat1-Requirements.xlsx
+++ b/CougSat1/CougSat1-Requirements.xlsx
@@ -5,17 +5,21 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bradley\Documents\CougsInSpace\CougSat1-Hardware\CougSat1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Bradley\Documents\CougsInSpace\CougSat1-Hardware\CougSat1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61538CBE-9B09-411D-8157-01802A7AAA75}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{851E0191-661F-40D3-9EFA-D633B8783B7B}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="1" r:id="rId1"/>
-    <sheet name="EPS" sheetId="3" r:id="rId2"/>
-    <sheet name="Old" sheetId="2" r:id="rId3"/>
+    <sheet name="C&amp;DH" sheetId="6" r:id="rId2"/>
+    <sheet name="EPS" sheetId="3" r:id="rId3"/>
+    <sheet name="ECS" sheetId="4" r:id="rId4"/>
+    <sheet name="IFJR" sheetId="7" r:id="rId5"/>
+    <sheet name="Structure" sheetId="5" r:id="rId6"/>
+    <sheet name="Old" sheetId="2" r:id="rId7"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -27,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="756" uniqueCount="318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="923" uniqueCount="409">
   <si>
     <t>CougSat-1 System Requirements</t>
   </si>
@@ -953,9 +957,6 @@
     <t>Independent power chains increases redundancy. Routing inputs/outputs allow load balancing and avoiding faulty components</t>
   </si>
   <si>
-    <t>The EPS shall have an regulated rail for the PMIC that is always on between the ejection from the P-POD for the mission duration</t>
-  </si>
-  <si>
     <t>The EPS shall be capable of entering safe mode where only critical subsystems are enabled</t>
   </si>
   <si>
@@ -981,6 +982,282 @@
   </si>
   <si>
     <t>CougSat-1 shall keep all components within prescribed operational temperature ranges beginning after ejection from the P-Pod for the mission duration</t>
+  </si>
+  <si>
+    <t>ECS Design Requirements</t>
+  </si>
+  <si>
+    <t>This sheet lists all of the design requirements of the satellite's ECS</t>
+  </si>
+  <si>
+    <t>ECS-001</t>
+  </si>
+  <si>
+    <t>ECS-002</t>
+  </si>
+  <si>
+    <t>ECS-003</t>
+  </si>
+  <si>
+    <t>The EPS shall have an regulated rail for the PMIC that is always on beginning after ejection from the P-Pod for the mission duration</t>
+  </si>
+  <si>
+    <t>REQ-009, REQ-022</t>
+  </si>
+  <si>
+    <t>Over and under temperature can stress components to failure</t>
+  </si>
+  <si>
+    <t>The ECS shall keep all components within storage temperature bounds</t>
+  </si>
+  <si>
+    <t>The ECS shall keep all components within operating temperature bounds beginning after ejection from the P-Pod for the mission duration</t>
+  </si>
+  <si>
+    <t>The ECS may protect against damaging levels of ionizing radiation</t>
+  </si>
+  <si>
+    <t>Ionizing radiation may result in damage to components</t>
+  </si>
+  <si>
+    <t>Structure Design Requirements</t>
+  </si>
+  <si>
+    <t>This sheet lists all of the design requirements of the satellite's Structure</t>
+  </si>
+  <si>
+    <t>STRUCT-001</t>
+  </si>
+  <si>
+    <t>STRUCT-002</t>
+  </si>
+  <si>
+    <t>STRUCT-003</t>
+  </si>
+  <si>
+    <t>STRUCT-004</t>
+  </si>
+  <si>
+    <t>STRUCT-005</t>
+  </si>
+  <si>
+    <t>STRUCT-006</t>
+  </si>
+  <si>
+    <t>The Structure shall mechanically support all subsystems</t>
+  </si>
+  <si>
+    <t>REQ-004, REQ-009</t>
+  </si>
+  <si>
+    <t>The subsystems cannot be ejected from the P-POD without being attached to rails</t>
+  </si>
+  <si>
+    <t>The Structure may maximize the use of commercial off-the-shelf parts</t>
+  </si>
+  <si>
+    <t>More things we can order, the less needs to be designed, fabricated, and tested</t>
+  </si>
+  <si>
+    <t>The Structure may limit the unique fasteners whenever the design allows</t>
+  </si>
+  <si>
+    <t>Using the same fastener is easier to design, fabricate, and assemble</t>
+  </si>
+  <si>
+    <t>The Structure may be used as a heatsink and radiation for the ECS</t>
+  </si>
+  <si>
+    <t>STRUCT-000</t>
+  </si>
+  <si>
+    <t>The Structure shall comply with all requirements listed below and all applicable system requirements</t>
+  </si>
+  <si>
+    <t>REQ-001, REQ-002, REQ-003, REQ-004, REQ-005, REQ-006, REQ-007, REQ-008, REQ-009, REQ-010, REQ-012, REQ-022, REQ-023, REQ-025, REQ-028, REQ-029</t>
+  </si>
+  <si>
+    <t>The Structure shall store deployables from before P-POD integration until controlled release from the EPS</t>
+  </si>
+  <si>
+    <t>The EPS shall activate deployables release mechanisms</t>
+  </si>
+  <si>
+    <t>EPS-023</t>
+  </si>
+  <si>
+    <t>Deployables release mechanism are high power devices requiring direct connection and control from the EPS</t>
+  </si>
+  <si>
+    <t>The deployables need to fit within the P-POD until the specified timeout after P-POD ejection</t>
+  </si>
+  <si>
+    <t>The Structure shall keep deployed deployables supported during slewing</t>
+  </si>
+  <si>
+    <t>REQ-009, REQ-023</t>
+  </si>
+  <si>
+    <t>The deployables cannot retractable and need to handle the dynamics induced from slewing</t>
+  </si>
+  <si>
+    <t>ECS-000</t>
+  </si>
+  <si>
+    <t>The ECS shall comply with all requirements listed below and all applicable system requirements</t>
+  </si>
+  <si>
+    <t>REQ-001, REQ-002, REQ-003, REQ-004, REQ-005, REQ-006, REQ-007, REQ-008, REQ-009, REQ-010, REQ-022, REQ-025, REQ-028, REQ-029</t>
+  </si>
+  <si>
+    <t>EPS-000</t>
+  </si>
+  <si>
+    <t>The EPS shall comply with all requirements listed below and all applicable system requirements</t>
+  </si>
+  <si>
+    <t>REQ-001, REQ-002, REQ-003, REQ-004, REQ-005, REQ-006, REQ-007, REQ-008, REQ-009, REQ-010, REQ-011, REQ-015, REQ-016, REQ-017, REQ-021, REQ-022, REQ-023, REQ-024, REQ-025, REQ-026, REQ-028, REQ-029, REQ-030</t>
+  </si>
+  <si>
+    <t>C&amp;DH Design Requirements</t>
+  </si>
+  <si>
+    <t>This sheet lists all of the design requirements of the satellite's C&amp;DH</t>
+  </si>
+  <si>
+    <t>CDH-000</t>
+  </si>
+  <si>
+    <t>CDH-001</t>
+  </si>
+  <si>
+    <t>CDH-002</t>
+  </si>
+  <si>
+    <t>CDH-003</t>
+  </si>
+  <si>
+    <t>CDH-004</t>
+  </si>
+  <si>
+    <t>CDH-005</t>
+  </si>
+  <si>
+    <t>CDH-006</t>
+  </si>
+  <si>
+    <t>CDH-007</t>
+  </si>
+  <si>
+    <t>CDH-008</t>
+  </si>
+  <si>
+    <t>CDH-009</t>
+  </si>
+  <si>
+    <t>CDH-010</t>
+  </si>
+  <si>
+    <t>The C&amp;DH shall comply with all requirements listed below and all applicable system requirements</t>
+  </si>
+  <si>
+    <t>REQ-001, REQ-002, REQ-003, REQ-004, REQ-005, REQ-006, REQ-007, REQ-008, REQ-009, REQ-010, REQ-011, REQ-014, REQ-015, REQ-016, REQ-017, REQ-021, REQ-025, REQ-026, REQ-028, REQ-029, REQ-030</t>
+  </si>
+  <si>
+    <t>The C&amp;DH shall have a single IHU</t>
+  </si>
+  <si>
+    <t>The C&amp;DH may manage all forms of data on the satellite</t>
+  </si>
+  <si>
+    <t>The C&amp;DH shall prepare all packets to send to the ground</t>
+  </si>
+  <si>
+    <t>The C&amp;DH shall interpret all packets received from the ground</t>
+  </si>
+  <si>
+    <t>The C&amp;DH shall collect and process information about all subsystems and payloads</t>
+  </si>
+  <si>
+    <t>The C&amp;DH shall keep and distribute the satellite's time with less or equal to one second resolution</t>
+  </si>
+  <si>
+    <t>The C&amp;DH shall have redundant non-volatile memory</t>
+  </si>
+  <si>
+    <t>The C&amp;DH shall execute all commands ordered by the ground</t>
+  </si>
+  <si>
+    <t>Heat may need to be absorbed or radiated by the structure to regulate subsystems' temperatures</t>
+  </si>
+  <si>
+    <t>The satellite need a single subsystem responsible for organizing all subsystems into a collective</t>
+  </si>
+  <si>
+    <t>Data needs to be buffered until it is used and not corrupted in the meanwhile</t>
+  </si>
+  <si>
+    <t>The C&amp;DH may decide and enforce current operation and mode</t>
+  </si>
+  <si>
+    <t>Synchronized time between all subsystems is required for time dependent operations</t>
+  </si>
+  <si>
+    <t>Different operations and modes need to affect all subsystems synchronously</t>
+  </si>
+  <si>
+    <t>The C&amp;DH shall perform periodic inquiries on the status of all subsystems</t>
+  </si>
+  <si>
+    <t>The subsystems may encouter a fault or be in critical health which requires the aid of other subsystems</t>
+  </si>
+  <si>
+    <t>REQ-011, REQ-016, REQ-021</t>
+  </si>
+  <si>
+    <t>REQ-009, REQ-011, REQ-016, REQ-021</t>
+  </si>
+  <si>
+    <t>REQ-014, REQ-015, REQ-026</t>
+  </si>
+  <si>
+    <t>IFJR Design Requirements</t>
+  </si>
+  <si>
+    <t>This sheet lists all of the design requirements of the satellite's IFJR</t>
+  </si>
+  <si>
+    <t>IFJR-000</t>
+  </si>
+  <si>
+    <t>IFJR-001</t>
+  </si>
+  <si>
+    <t>IFJR-002</t>
+  </si>
+  <si>
+    <t>IFJR-003</t>
+  </si>
+  <si>
+    <t>IFJR-004</t>
+  </si>
+  <si>
+    <t>IFJR-005</t>
+  </si>
+  <si>
+    <t>IFJR-006</t>
+  </si>
+  <si>
+    <t>IFJR-007</t>
+  </si>
+  <si>
+    <t>IFJR-008</t>
+  </si>
+  <si>
+    <t>IFJR-009</t>
+  </si>
+  <si>
+    <t>IFJR-010</t>
   </si>
 </sst>
 </file>
@@ -1044,28 +1321,28 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1384,30 +1661,30 @@
   <dimension ref="A1:G79"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B26" sqref="B26"/>
+      <pane ySplit="3" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.140625" style="10" customWidth="1"/>
-    <col min="2" max="2" width="78.85546875" style="13" customWidth="1"/>
-    <col min="3" max="3" width="60.5703125" style="13" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.42578125" style="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="10"/>
+    <col min="1" max="1" width="10.140625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="78.85546875" style="9" customWidth="1"/>
+    <col min="3" max="3" width="60.5703125" style="9" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
@@ -1417,8 +1694,8 @@
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
     </row>
     <row r="3" spans="1:7" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
@@ -1438,889 +1715,889 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="7" t="s">
         <v>219</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="9" t="s">
         <v>220</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="9" t="s">
         <v>221</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="9" t="s">
         <v>192</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="9" t="s">
         <v>193</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="E5" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="9" t="s">
         <v>222</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="9" t="s">
         <v>223</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="E7" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="9" t="s">
         <v>224</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="E8" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="9" t="s">
         <v>225</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D9" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="E9" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="9" t="s">
         <v>226</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="D10" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="E10" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="B11" s="13" t="s">
+      <c r="B11" s="9" t="s">
         <v>227</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="D11" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="E11" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="10" t="s">
+      <c r="A12" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="B12" s="13" t="s">
+      <c r="B12" s="9" t="s">
         <v>228</v>
       </c>
-      <c r="C12" s="13" t="s">
+      <c r="C12" s="9" t="s">
         <v>229</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="D12" s="7" t="s">
         <v>230</v>
       </c>
-      <c r="E12" s="10" t="s">
+      <c r="E12" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="10" t="s">
+      <c r="A13" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="B13" s="13" t="s">
+      <c r="B13" s="9" t="s">
         <v>231</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="C13" s="9" t="s">
         <v>229</v>
       </c>
-      <c r="D13" s="10" t="s">
+      <c r="D13" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="E13" s="10" t="s">
+      <c r="E13" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="10" t="s">
+      <c r="A14" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="B14" s="13" t="s">
+      <c r="B14" s="9" t="s">
         <v>232</v>
       </c>
-      <c r="C14" s="13" t="s">
+      <c r="C14" s="9" t="s">
         <v>233</v>
       </c>
-      <c r="D14" s="10" t="s">
+      <c r="D14" s="7" t="s">
         <v>230</v>
       </c>
-      <c r="E14" s="10" t="s">
+      <c r="E14" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="10" t="s">
+      <c r="A15" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B15" s="13" t="s">
+      <c r="B15" s="9" t="s">
         <v>234</v>
       </c>
-      <c r="C15" s="13" t="s">
+      <c r="C15" s="9" t="s">
         <v>235</v>
       </c>
-      <c r="D15" s="10" t="s">
+      <c r="D15" s="7" t="s">
         <v>230</v>
       </c>
-      <c r="E15" s="10" t="s">
+      <c r="E15" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="10" t="s">
+      <c r="A16" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B16" s="13" t="s">
+      <c r="B16" s="9" t="s">
         <v>236</v>
       </c>
-      <c r="C16" s="13" t="s">
+      <c r="C16" s="9" t="s">
         <v>237</v>
       </c>
-      <c r="D16" s="10" t="s">
+      <c r="D16" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="E16" s="10" t="s">
+      <c r="E16" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="10" t="s">
+      <c r="A17" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="B17" s="13" t="s">
+      <c r="B17" s="9" t="s">
         <v>238</v>
       </c>
-      <c r="C17" s="13" t="s">
+      <c r="C17" s="9" t="s">
         <v>182</v>
       </c>
-      <c r="D17" s="10" t="s">
+      <c r="D17" s="7" t="s">
         <v>239</v>
       </c>
-      <c r="E17" s="10" t="s">
+      <c r="E17" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="10" t="s">
+      <c r="A18" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="B18" s="13" t="s">
+      <c r="B18" s="9" t="s">
+        <v>313</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>240</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>241</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>242</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>240</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>243</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>244</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>245</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>246</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B23" s="9" t="s">
         <v>314</v>
       </c>
-      <c r="C18" s="13" t="s">
-        <v>240</v>
-      </c>
-      <c r="D18" s="10" t="s">
+      <c r="C23" s="9" t="s">
+        <v>315</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>247</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>248</v>
+      </c>
+      <c r="D24" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="E18" s="10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="B19" s="13" t="s">
-        <v>241</v>
-      </c>
-      <c r="C19" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="D19" s="10" t="s">
+      <c r="E24" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>249</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="D25" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="E19" s="10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="B20" s="13" t="s">
-        <v>242</v>
-      </c>
-      <c r="C20" s="13" t="s">
-        <v>240</v>
-      </c>
-      <c r="D20" s="10" t="s">
+      <c r="E25" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>316</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>250</v>
+      </c>
+      <c r="D26" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="E20" s="10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="B21" s="13" t="s">
-        <v>243</v>
-      </c>
-      <c r="C21" s="13" t="s">
-        <v>244</v>
-      </c>
-      <c r="D21" s="10" t="s">
+      <c r="E26" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>251</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>252</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>253</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>254</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>255</v>
+      </c>
+      <c r="D29" s="7" t="s">
         <v>230</v>
       </c>
-      <c r="E21" s="10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="B22" s="13" t="s">
-        <v>245</v>
-      </c>
-      <c r="C22" s="13" t="s">
-        <v>246</v>
-      </c>
-      <c r="D22" s="10" t="s">
+      <c r="E29" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>256</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>311</v>
+      </c>
+      <c r="D30" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="E22" s="10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="B23" s="13" t="s">
-        <v>315</v>
-      </c>
-      <c r="C23" s="13" t="s">
-        <v>316</v>
-      </c>
-      <c r="D23" s="10" t="s">
+      <c r="E30" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>258</v>
+      </c>
+      <c r="D31" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="E31" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>259</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>260</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="E32" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>261</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="D33" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="E33" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>312</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>262</v>
+      </c>
+      <c r="D34" s="7" t="s">
         <v>230</v>
       </c>
-      <c r="E23" s="10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="B24" s="13" t="s">
-        <v>247</v>
-      </c>
-      <c r="C24" s="13" t="s">
-        <v>248</v>
-      </c>
-      <c r="D24" s="10" t="s">
-        <v>194</v>
-      </c>
-      <c r="E24" s="10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="B25" s="13" t="s">
-        <v>249</v>
-      </c>
-      <c r="C25" s="13" t="s">
-        <v>229</v>
-      </c>
-      <c r="D25" s="10" t="s">
-        <v>194</v>
-      </c>
-      <c r="E25" s="10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="B26" s="13" t="s">
-        <v>317</v>
-      </c>
-      <c r="C26" s="13" t="s">
-        <v>250</v>
-      </c>
-      <c r="D26" s="10" t="s">
-        <v>194</v>
-      </c>
-      <c r="E26" s="10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="B27" s="13" t="s">
-        <v>251</v>
-      </c>
-      <c r="C27" s="13" t="s">
-        <v>252</v>
-      </c>
-      <c r="D27" s="10" t="s">
-        <v>194</v>
-      </c>
-      <c r="E27" s="10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="B28" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="C28" s="13" t="s">
-        <v>159</v>
-      </c>
-      <c r="D28" s="10" t="s">
-        <v>194</v>
-      </c>
-      <c r="E28" s="10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="B29" s="13" t="s">
-        <v>254</v>
-      </c>
-      <c r="C29" s="13" t="s">
-        <v>255</v>
-      </c>
-      <c r="D29" s="10" t="s">
-        <v>230</v>
-      </c>
-      <c r="E29" s="10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="B30" s="13" t="s">
-        <v>256</v>
-      </c>
-      <c r="C30" s="13" t="s">
-        <v>312</v>
-      </c>
-      <c r="D30" s="10" t="s">
-        <v>194</v>
-      </c>
-      <c r="E30" s="10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="B31" s="13" t="s">
-        <v>257</v>
-      </c>
-      <c r="C31" s="13" t="s">
-        <v>258</v>
-      </c>
-      <c r="D31" s="10" t="s">
-        <v>194</v>
-      </c>
-      <c r="E31" s="10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="B32" s="13" t="s">
-        <v>259</v>
-      </c>
-      <c r="C32" s="13" t="s">
-        <v>260</v>
-      </c>
-      <c r="D32" s="10" t="s">
-        <v>194</v>
-      </c>
-      <c r="E32" s="10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="B33" s="13" t="s">
-        <v>261</v>
-      </c>
-      <c r="C33" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="D33" s="10" t="s">
-        <v>194</v>
-      </c>
-      <c r="E33" s="10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="B34" s="13" t="s">
-        <v>313</v>
-      </c>
-      <c r="C34" s="13" t="s">
-        <v>262</v>
-      </c>
-      <c r="D34" s="10" t="s">
-        <v>230</v>
-      </c>
-      <c r="E34" s="10" t="s">
+      <c r="E34" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="10" t="s">
+      <c r="A35" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="E35" s="10" t="s">
+      <c r="E35" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="10" t="s">
+      <c r="A36" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="E36" s="10" t="s">
+      <c r="E36" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="10" t="s">
+      <c r="A37" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="E37" s="10" t="s">
+      <c r="E37" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="10" t="s">
+      <c r="A38" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="E38" s="10" t="s">
+      <c r="E38" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="10" t="s">
+      <c r="A39" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="E39" s="10" t="s">
+      <c r="E39" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="10" t="s">
+      <c r="A40" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="E40" s="10" t="s">
+      <c r="E40" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="10" t="s">
+      <c r="A41" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="E41" s="10" t="s">
+      <c r="E41" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="10" t="s">
+      <c r="A42" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="E42" s="10" t="s">
+      <c r="E42" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="10" t="s">
+      <c r="A43" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="E43" s="10" t="s">
+      <c r="E43" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="10" t="s">
+      <c r="A44" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="E44" s="10" t="s">
+      <c r="E44" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="10" t="s">
+      <c r="A45" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="E45" s="10" t="s">
+      <c r="E45" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="10" t="s">
+      <c r="A46" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="E46" s="10" t="s">
+      <c r="E46" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="10" t="s">
+      <c r="A47" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="E47" s="10" t="s">
+      <c r="E47" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="10" t="s">
+      <c r="A48" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="E48" s="10" t="s">
+      <c r="E48" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="10" t="s">
+      <c r="A49" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="E49" s="10" t="s">
+      <c r="E49" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="10" t="s">
+      <c r="A50" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="E50" s="10" t="s">
+      <c r="E50" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="10" t="s">
+      <c r="A51" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="E51" s="10" t="s">
+      <c r="E51" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="10" t="s">
+      <c r="A52" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="E52" s="10" t="s">
+      <c r="E52" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="10" t="s">
+      <c r="A53" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="E53" s="10" t="s">
+      <c r="E53" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="10" t="s">
+      <c r="A54" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="E54" s="10" t="s">
+      <c r="E54" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="10" t="s">
+      <c r="A55" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="E55" s="10" t="s">
+      <c r="E55" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="10" t="s">
+      <c r="A56" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="E56" s="10" t="s">
+      <c r="E56" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="10" t="s">
+      <c r="A57" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="E57" s="10" t="s">
+      <c r="E57" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="10" t="s">
+      <c r="A58" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="E58" s="10" t="s">
+      <c r="E58" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" s="10" t="s">
+      <c r="A59" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="E59" s="10" t="s">
+      <c r="E59" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" s="10" t="s">
+      <c r="A60" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="E60" s="10" t="s">
+      <c r="E60" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61" s="10" t="s">
+      <c r="A61" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="E61" s="10" t="s">
+      <c r="E61" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" s="10" t="s">
+      <c r="A62" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="E62" s="10" t="s">
+      <c r="E62" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A63" s="10" t="s">
+      <c r="A63" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="E63" s="10" t="s">
+      <c r="E63" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A64" s="10" t="s">
+      <c r="A64" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="E64" s="10" t="s">
+      <c r="E64" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A65" s="10" t="s">
+      <c r="A65" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="E65" s="10" t="s">
+      <c r="E65" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" s="10" t="s">
+      <c r="A66" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="E66" s="10" t="s">
+      <c r="E66" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67" s="10" t="s">
+      <c r="A67" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="E67" s="10" t="s">
+      <c r="E67" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" s="10" t="s">
+      <c r="A68" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="E68" s="10" t="s">
+      <c r="E68" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A69" s="10" t="s">
+      <c r="A69" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="E69" s="10" t="s">
+      <c r="E69" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70" s="10" t="s">
+      <c r="A70" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="E70" s="10" t="s">
+      <c r="E70" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A71" s="10" t="s">
+      <c r="A71" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="E71" s="10" t="s">
+      <c r="E71" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A72" s="10" t="s">
+      <c r="A72" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="E72" s="10" t="s">
+      <c r="E72" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A73" s="10" t="s">
+      <c r="A73" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="E73" s="10" t="s">
+      <c r="E73" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A74" s="10" t="s">
+      <c r="A74" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="E74" s="10" t="s">
+      <c r="E74" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A75" s="10" t="s">
+      <c r="A75" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="E75" s="10" t="s">
+      <c r="E75" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A76" s="10" t="s">
+      <c r="A76" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="E76" s="10" t="s">
+      <c r="E76" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A77" s="10" t="s">
+      <c r="A77" s="7" t="s">
         <v>184</v>
       </c>
-      <c r="E77" s="10" t="s">
+      <c r="E77" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A78" s="10" t="s">
+      <c r="A78" s="7" t="s">
         <v>188</v>
       </c>
-      <c r="E78" s="10" t="s">
+      <c r="E78" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A79" s="10" t="s">
+      <c r="A79" s="7" t="s">
         <v>189</v>
       </c>
-      <c r="E79" s="10" t="s">
+      <c r="E79" s="7" t="s">
         <v>9</v>
       </c>
     </row>
@@ -2335,45 +2612,44 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D8478C5-1713-4B9E-8DAE-5F54C2737D56}">
-  <dimension ref="A1:G25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30B4B5ED-6412-48B2-94ED-1EEF687C55DD}">
+  <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E26" sqref="E26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.140625" style="10" customWidth="1"/>
-    <col min="2" max="2" width="72.28515625" style="13" customWidth="1"/>
-    <col min="3" max="3" width="59.140625" style="13" customWidth="1"/>
-    <col min="4" max="4" width="26.140625" style="13" customWidth="1"/>
-    <col min="5" max="5" width="9.42578125" style="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="10"/>
+    <col min="1" max="1" width="10.140625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="72.28515625" style="9" customWidth="1"/>
+    <col min="3" max="3" width="59.140625" style="9" customWidth="1"/>
+    <col min="4" max="4" width="26.140625" style="9" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
-        <v>195</v>
-      </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
+      <c r="A1" s="10" t="s">
+        <v>362</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
-        <v>196</v>
+        <v>363</v>
       </c>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
     </row>
     <row r="3" spans="1:7" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
@@ -2392,377 +2668,190 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
-        <v>197</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>263</v>
-      </c>
-      <c r="C4" s="13" t="s">
-        <v>264</v>
-      </c>
-      <c r="D4" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="E4" s="10" t="s">
+    <row r="4" spans="1:7" s="5" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>364</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>375</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>221</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>376</v>
+      </c>
+      <c r="E4" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
-        <v>198</v>
-      </c>
-      <c r="B5" s="13" t="s">
-        <v>267</v>
-      </c>
-      <c r="C5" s="13" t="s">
-        <v>265</v>
-      </c>
-      <c r="D5" s="13" t="s">
+      <c r="A5" s="7" t="s">
+        <v>365</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>377</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>303</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>275</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>366</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>378</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>386</v>
+      </c>
+      <c r="D6" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="E5" s="10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
-        <v>199</v>
-      </c>
-      <c r="B6" s="13" t="s">
-        <v>269</v>
-      </c>
-      <c r="C6" s="13" t="s">
-        <v>266</v>
-      </c>
-      <c r="D6" s="13" t="s">
+      <c r="E6" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>367</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>384</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>386</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>368</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>379</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>386</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>393</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>369</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>380</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>386</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>370</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>381</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>386</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>394</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>371</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>382</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>389</v>
+      </c>
+      <c r="D11" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="E6" s="10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
-        <v>200</v>
-      </c>
-      <c r="B7" s="13" t="s">
-        <v>268</v>
-      </c>
-      <c r="C7" s="13" t="s">
-        <v>266</v>
-      </c>
-      <c r="D7" s="13" t="s">
+      <c r="E11" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>372</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>383</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>387</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>395</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>373</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>388</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>390</v>
+      </c>
+      <c r="D13" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="E7" s="10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
-        <v>201</v>
-      </c>
-      <c r="B8" s="13" t="s">
-        <v>273</v>
-      </c>
-      <c r="C8" s="13" t="s">
-        <v>270</v>
-      </c>
-      <c r="D8" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
-        <v>202</v>
-      </c>
-      <c r="B9" s="13" t="s">
-        <v>271</v>
-      </c>
-      <c r="C9" s="13" t="s">
-        <v>272</v>
-      </c>
-      <c r="D9" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="10" t="s">
-        <v>203</v>
-      </c>
-      <c r="B10" s="13" t="s">
-        <v>305</v>
-      </c>
-      <c r="C10" s="13" t="s">
-        <v>274</v>
-      </c>
-      <c r="D10" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="10" t="s">
-        <v>204</v>
-      </c>
-      <c r="B11" s="13" t="s">
-        <v>306</v>
-      </c>
-      <c r="C11" s="13" t="s">
-        <v>307</v>
-      </c>
-      <c r="D11" s="13" t="s">
+      <c r="E13" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
+        <v>374</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>391</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>392</v>
+      </c>
+      <c r="D14" s="9" t="s">
         <v>275</v>
       </c>
-      <c r="E11" s="10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="10" t="s">
-        <v>205</v>
-      </c>
-      <c r="B12" s="13" t="s">
-        <v>276</v>
-      </c>
-      <c r="C12" s="13" t="s">
-        <v>277</v>
-      </c>
-      <c r="D12" s="13" t="s">
-        <v>278</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="10" t="s">
-        <v>206</v>
-      </c>
-      <c r="B13" s="13" t="s">
-        <v>279</v>
-      </c>
-      <c r="C13" s="13" t="s">
-        <v>280</v>
-      </c>
-      <c r="D13" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="10" t="s">
-        <v>207</v>
-      </c>
-      <c r="B14" s="13" t="s">
-        <v>281</v>
-      </c>
-      <c r="C14" s="13" t="s">
-        <v>282</v>
-      </c>
-      <c r="D14" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="10" t="s">
-        <v>208</v>
-      </c>
-      <c r="B15" s="13" t="s">
-        <v>283</v>
-      </c>
-      <c r="C15" s="13" t="s">
-        <v>284</v>
-      </c>
-      <c r="D15" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="E15" s="10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="10" t="s">
-        <v>209</v>
-      </c>
-      <c r="B16" s="13" t="s">
-        <v>308</v>
-      </c>
-      <c r="C16" s="13" t="s">
-        <v>285</v>
-      </c>
-      <c r="D16" s="13" t="s">
-        <v>286</v>
-      </c>
-      <c r="E16" s="10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="10" t="s">
-        <v>210</v>
-      </c>
-      <c r="B17" s="13" t="s">
-        <v>309</v>
-      </c>
-      <c r="C17" s="13" t="s">
-        <v>287</v>
-      </c>
-      <c r="D17" s="13" t="s">
-        <v>288</v>
-      </c>
-      <c r="E17" s="10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="10" t="s">
-        <v>211</v>
-      </c>
-      <c r="B18" s="13" t="s">
-        <v>289</v>
-      </c>
-      <c r="C18" s="13" t="s">
-        <v>293</v>
-      </c>
-      <c r="D18" s="13" t="s">
-        <v>292</v>
-      </c>
-      <c r="E18" s="10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="10" t="s">
-        <v>212</v>
-      </c>
-      <c r="B19" s="13" t="s">
-        <v>290</v>
-      </c>
-      <c r="C19" s="13" t="s">
-        <v>294</v>
-      </c>
-      <c r="D19" s="13" t="s">
-        <v>292</v>
-      </c>
-      <c r="E19" s="10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="10" t="s">
-        <v>213</v>
-      </c>
-      <c r="B20" s="13" t="s">
-        <v>291</v>
-      </c>
-      <c r="C20" s="13" t="s">
-        <v>310</v>
-      </c>
-      <c r="D20" s="13" t="s">
-        <v>292</v>
-      </c>
-      <c r="E20" s="10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="10" t="s">
-        <v>214</v>
-      </c>
-      <c r="B21" s="13" t="s">
-        <v>295</v>
-      </c>
-      <c r="C21" s="13" t="s">
-        <v>296</v>
-      </c>
-      <c r="D21" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="E21" s="10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="10" t="s">
-        <v>215</v>
-      </c>
-      <c r="B22" s="13" t="s">
-        <v>297</v>
-      </c>
-      <c r="C22" s="13" t="s">
-        <v>298</v>
-      </c>
-      <c r="D22" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="E22" s="10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="10" t="s">
-        <v>216</v>
-      </c>
-      <c r="B23" s="13" t="s">
-        <v>299</v>
-      </c>
-      <c r="C23" s="13" t="s">
-        <v>300</v>
-      </c>
-      <c r="D23" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="E23" s="10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="10" t="s">
-        <v>217</v>
-      </c>
-      <c r="B24" s="13" t="s">
-        <v>301</v>
-      </c>
-      <c r="C24" s="13" t="s">
-        <v>311</v>
-      </c>
-      <c r="D24" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="E24" s="10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="10" t="s">
-        <v>218</v>
-      </c>
-      <c r="B25" s="13" t="s">
-        <v>302</v>
-      </c>
-      <c r="C25" s="13" t="s">
-        <v>303</v>
-      </c>
-      <c r="D25" s="13" t="s">
-        <v>275</v>
-      </c>
-      <c r="E25" s="10" t="s">
+      <c r="E14" s="7" t="s">
         <v>9</v>
       </c>
     </row>
@@ -2776,6 +2865,949 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D8478C5-1713-4B9E-8DAE-5F54C2737D56}">
+  <dimension ref="A1:G27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B25" sqref="B25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.140625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="72.28515625" style="9" customWidth="1"/>
+    <col min="3" max="3" width="59.140625" style="9" customWidth="1"/>
+    <col min="4" max="4" width="26.140625" style="9" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>195</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
+        <v>196</v>
+      </c>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+    </row>
+    <row r="3" spans="1:7" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" s="5" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>359</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>360</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>221</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>361</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>263</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>264</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>267</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>265</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>269</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>266</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>268</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>266</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>273</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>270</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>271</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>272</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>305</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>274</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>204</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>306</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>307</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>275</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>276</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>278</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>279</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>280</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>281</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>282</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
+        <v>208</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>283</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>284</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>322</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>285</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>286</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>287</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>288</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>289</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>293</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>290</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>294</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>291</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>309</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>295</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>296</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>297</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>298</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>299</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>300</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>301</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>310</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="7" t="s">
+        <v>218</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>302</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>303</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>275</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="7" t="s">
+        <v>350</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>349</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>351</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A2:E2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AD803A9-AF18-4300-9C9D-F24D7CF02CCF}">
+  <dimension ref="A1:G7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.140625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="72.28515625" style="9" customWidth="1"/>
+    <col min="3" max="3" width="59.140625" style="9" customWidth="1"/>
+    <col min="4" max="4" width="26.140625" style="9" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>317</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
+        <v>318</v>
+      </c>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+    </row>
+    <row r="3" spans="1:7" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" s="5" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>356</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>357</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>221</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>358</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>319</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>325</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>324</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>323</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>320</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>326</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>324</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>323</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>321</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>327</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>328</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A2:E2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5083188-FC9C-4563-81AC-AF6CFA6582AC}">
+  <dimension ref="A1:G14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.140625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="72.28515625" style="9" customWidth="1"/>
+    <col min="3" max="3" width="59.140625" style="9" customWidth="1"/>
+    <col min="4" max="4" width="26.140625" style="9" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>396</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
+        <v>397</v>
+      </c>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+    </row>
+    <row r="3" spans="1:7" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" s="5" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>398</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>375</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>221</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>376</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>399</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>377</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>303</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>275</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
+        <v>408</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A2:E2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D14F67A4-A4C6-4846-971E-9E85D1BD727D}">
+  <dimension ref="A1:G10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="72.28515625" style="9" customWidth="1"/>
+    <col min="3" max="3" width="59.140625" style="9" customWidth="1"/>
+    <col min="4" max="4" width="26.140625" style="9" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>329</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
+        <v>330</v>
+      </c>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+    </row>
+    <row r="3" spans="1:7" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" s="5" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>345</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>346</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>221</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>347</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>331</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>337</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>339</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>338</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>332</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>340</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>341</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>333</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>342</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>343</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>334</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>344</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>385</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>335</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>348</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>352</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>336</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>353</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>355</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>354</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A2:E2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65935663-0434-49C2-B8D3-B1FF868B4552}">
   <dimension ref="A1:G79"/>
   <sheetViews>
@@ -2793,24 +3825,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
     </row>

</xml_diff>

<commit_message>
Wrote Comms Design Requirements
</commit_message>
<xml_diff>
--- a/CougSat1/CougSat1-Requirements.xlsx
+++ b/CougSat1/CougSat1-Requirements.xlsx
@@ -1,27 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Bradley\Documents\CougsInSpace\CougSat1-Hardware\CougSat1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{851E0191-661F-40D3-9EFA-D633B8783B7B}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA90D291-8EFB-498C-89D7-C14B47753FBF}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="1" r:id="rId1"/>
-    <sheet name="C&amp;DH" sheetId="6" r:id="rId2"/>
-    <sheet name="EPS" sheetId="3" r:id="rId3"/>
-    <sheet name="ECS" sheetId="4" r:id="rId4"/>
-    <sheet name="IFJR" sheetId="7" r:id="rId5"/>
-    <sheet name="Structure" sheetId="5" r:id="rId6"/>
-    <sheet name="Old" sheetId="2" r:id="rId7"/>
+    <sheet name="ADCS" sheetId="9" r:id="rId2"/>
+    <sheet name="C&amp;DH" sheetId="6" r:id="rId3"/>
+    <sheet name="Comms" sheetId="8" r:id="rId4"/>
+    <sheet name="EPS" sheetId="3" r:id="rId5"/>
+    <sheet name="ECS" sheetId="4" r:id="rId6"/>
+    <sheet name="IFJR" sheetId="7" r:id="rId7"/>
+    <sheet name="Payload" sheetId="10" r:id="rId8"/>
+    <sheet name="Structure" sheetId="5" r:id="rId9"/>
+    <sheet name="Old" sheetId="2" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="923" uniqueCount="409">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1000" uniqueCount="454">
   <si>
     <t>CougSat-1 System Requirements</t>
   </si>
@@ -1242,22 +1245,157 @@
     <t>IFJR-004</t>
   </si>
   <si>
-    <t>IFJR-005</t>
-  </si>
-  <si>
-    <t>IFJR-006</t>
-  </si>
-  <si>
-    <t>IFJR-007</t>
-  </si>
-  <si>
-    <t>IFJR-008</t>
-  </si>
-  <si>
-    <t>IFJR-009</t>
-  </si>
-  <si>
-    <t>IFJR-010</t>
+    <t>Comms Design Requirements</t>
+  </si>
+  <si>
+    <t>This sheet lists all of the design requirements of the satellite's Comms</t>
+  </si>
+  <si>
+    <t>COMMS-000</t>
+  </si>
+  <si>
+    <t>COMMS-001</t>
+  </si>
+  <si>
+    <t>COMMS-002</t>
+  </si>
+  <si>
+    <t>COMMS-003</t>
+  </si>
+  <si>
+    <t>COMMS-004</t>
+  </si>
+  <si>
+    <t>COMMS-005</t>
+  </si>
+  <si>
+    <t>COMMS-006</t>
+  </si>
+  <si>
+    <t>COMMS-007</t>
+  </si>
+  <si>
+    <t>The Comms shall comply with all requirements listed below and all applicable system requirements</t>
+  </si>
+  <si>
+    <t>The IFJR shall comply with all requirements listed below and all applicable system requirements</t>
+  </si>
+  <si>
+    <t>REQ-001, REQ-002, REQ-003, REQ-004, REQ-005, REQ-006, REQ-007, REQ-008, REQ-009, REQ-014, REQ-015, REQ-016, REQ-017, REQ-021, REQ-025, REQ-026, REQ-028, REQ-029</t>
+  </si>
+  <si>
+    <t>The IFJR shall have a single processor</t>
+  </si>
+  <si>
+    <t>The IFJR may program any subsystem processor using JTAG</t>
+  </si>
+  <si>
+    <t>JTAG programming is widely used and is not complex to implement</t>
+  </si>
+  <si>
+    <t>The IFJR shall alert a subsytem before performing programming operations</t>
+  </si>
+  <si>
+    <t>Sudden programming can interupt a CMT</t>
+  </si>
+  <si>
+    <t>The IFJR shall have redundant non-volatile memory</t>
+  </si>
+  <si>
+    <t>Processor binaries needs to be buffered until it is used and not corrupted in the meanwhile</t>
+  </si>
+  <si>
+    <t>REQ-009, REQ-017</t>
+  </si>
+  <si>
+    <t>REQ-014, REQ-015</t>
+  </si>
+  <si>
+    <t>REQ-001, REQ-002, REQ-003, REQ-004, REQ-005, REQ-006, REQ-007, REQ-008, REQ-009, REQ-010, REQ-011, REQ-013, REQ-014, REQ-015, REQ-016, REQ-017, REQ-021, REQ-022, REQ-023, REQ-025, REQ-026, REQ-028, REQ-029, REQ-030</t>
+  </si>
+  <si>
+    <t>CW is the most spectrum efficient, can get through the weakest link, and lowest power consumption transmission</t>
+  </si>
+  <si>
+    <t>The Comms shall have a CW beacon during SAFE mode and only after the specified radio inhibit timeout</t>
+  </si>
+  <si>
+    <t>The Comms shall have a telemetry containing beacon during STANDBY and SCIENCE mode and only after the specified radio inhibit timeout</t>
+  </si>
+  <si>
+    <t>The beacon will be used for tracking and will send telemetry to any ground station</t>
+  </si>
+  <si>
+    <t>The Comms may have a high speed downlink during TRANSMIT mode and only after the specified radio inhibit timeout capable of at least 500kbps goodput</t>
+  </si>
+  <si>
+    <t>This will be used to transfer large files (payload images). A single photo will take 80s at this rate which is up to 30 images a day</t>
+  </si>
+  <si>
+    <t>Communication from the ground may occur at any time</t>
+  </si>
+  <si>
+    <t>The Comms may have a voice message audible during the telemetry beacon</t>
+  </si>
+  <si>
+    <t>Listener can be informed of our website which will have instructions for decoding the telemetry encoded in the transmission</t>
+  </si>
+  <si>
+    <t>REQ-009, REQ-014, REQ-016</t>
+  </si>
+  <si>
+    <t>REQ-009, REQ-014, REQ-016, REQ-021</t>
+  </si>
+  <si>
+    <t>REQ-011, REQ-014, REQ-016, REQ-017, REQ-021</t>
+  </si>
+  <si>
+    <t>REQ-009, REQ-014</t>
+  </si>
+  <si>
+    <t>REQ-009, REQ-014, REQ-020</t>
+  </si>
+  <si>
+    <t>The Comms shall have at least a low gain antenna</t>
+  </si>
+  <si>
+    <t>If the ADCS malfunctions, data still needs to be capable of transferring to the ground (low gain is low directionality)</t>
+  </si>
+  <si>
+    <t>The Comms shall have sufficient preamble for receiver synchronization</t>
+  </si>
+  <si>
+    <t>A preamble allows the receiver to wake up and recover the clock from the signal</t>
+  </si>
+  <si>
+    <t>The Comms shall have a receiver continuously on and only after the specified radio inhibit timeout</t>
+  </si>
+  <si>
+    <t>ADCS Design Requirements</t>
+  </si>
+  <si>
+    <t>This sheet lists all of the design requirements of the satellite's ADCS</t>
+  </si>
+  <si>
+    <t>The ADCS shall comply with all requirements listed below and all applicable system requirements</t>
+  </si>
+  <si>
+    <t>ADCS-000</t>
+  </si>
+  <si>
+    <t>Payload Design Requirements</t>
+  </si>
+  <si>
+    <t>This sheet lists all of the design requirements of the satellite's Payload</t>
+  </si>
+  <si>
+    <t>PAYLOAD-000</t>
+  </si>
+  <si>
+    <t>The Payload shall comply with all requirements listed below and all applicable system requirements</t>
+  </si>
+  <si>
+    <t>REQ-001, REQ-002, REQ-003, REQ-004, REQ-005, REQ-006, REQ-007, REQ-008, REQ-009, REQ-010, REQ-011, REQ-014, REQ-015, REQ-016, REQ-022, REQ-023, REQ-025, REQ-026, REQ-028, REQ-029, REQ-030</t>
   </si>
 </sst>
 </file>
@@ -2611,12 +2749,1452 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65935663-0434-49C2-B8D3-B1FF868B4552}">
+  <dimension ref="A1:G79"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.140625" customWidth="1"/>
+    <col min="2" max="2" width="72.28515625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="50.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+    </row>
+    <row r="3" spans="1:7" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E20" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" t="s">
+        <v>11</v>
+      </c>
+      <c r="E21" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" t="s">
+        <v>11</v>
+      </c>
+      <c r="E22" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D23" t="s">
+        <v>11</v>
+      </c>
+      <c r="E23" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D24" t="s">
+        <v>11</v>
+      </c>
+      <c r="E24" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D25" t="s">
+        <v>11</v>
+      </c>
+      <c r="E25" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D26" t="s">
+        <v>11</v>
+      </c>
+      <c r="E26" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D27" t="s">
+        <v>11</v>
+      </c>
+      <c r="E27" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D28" t="s">
+        <v>11</v>
+      </c>
+      <c r="E28" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D29" t="s">
+        <v>11</v>
+      </c>
+      <c r="E29" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D30" t="s">
+        <v>11</v>
+      </c>
+      <c r="E30" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D31" t="s">
+        <v>11</v>
+      </c>
+      <c r="E31" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D32" t="s">
+        <v>11</v>
+      </c>
+      <c r="E32" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D33" t="s">
+        <v>11</v>
+      </c>
+      <c r="E33" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D34" t="s">
+        <v>11</v>
+      </c>
+      <c r="E34" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D35" t="s">
+        <v>11</v>
+      </c>
+      <c r="E35" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D36" t="s">
+        <v>11</v>
+      </c>
+      <c r="E36" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D37" t="s">
+        <v>11</v>
+      </c>
+      <c r="E37" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D38" t="s">
+        <v>11</v>
+      </c>
+      <c r="E38" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D39" t="s">
+        <v>11</v>
+      </c>
+      <c r="E39" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D40" t="s">
+        <v>11</v>
+      </c>
+      <c r="E40" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D41" t="s">
+        <v>11</v>
+      </c>
+      <c r="E41" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D42" t="s">
+        <v>11</v>
+      </c>
+      <c r="E42" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D43" t="s">
+        <v>11</v>
+      </c>
+      <c r="E43" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D44" t="s">
+        <v>11</v>
+      </c>
+      <c r="E44" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D45" t="s">
+        <v>11</v>
+      </c>
+      <c r="E45" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D46" t="s">
+        <v>11</v>
+      </c>
+      <c r="E46" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D47" t="s">
+        <v>11</v>
+      </c>
+      <c r="E47" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D48" t="s">
+        <v>11</v>
+      </c>
+      <c r="E48" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="D49" t="s">
+        <v>93</v>
+      </c>
+      <c r="E49" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="D50" t="s">
+        <v>93</v>
+      </c>
+      <c r="E50" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="D51" t="s">
+        <v>93</v>
+      </c>
+      <c r="E51" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="D52" t="s">
+        <v>11</v>
+      </c>
+      <c r="E52" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="D53" t="s">
+        <v>93</v>
+      </c>
+      <c r="E53" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="D54" t="s">
+        <v>93</v>
+      </c>
+      <c r="E54" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="D55" t="s">
+        <v>93</v>
+      </c>
+      <c r="E55" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="D56" t="s">
+        <v>11</v>
+      </c>
+      <c r="E56" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="D57" t="s">
+        <v>11</v>
+      </c>
+      <c r="E57" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="B58" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="D58" t="s">
+        <v>93</v>
+      </c>
+      <c r="E58" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A59" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="D59" t="s">
+        <v>93</v>
+      </c>
+      <c r="E59" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B60" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="C60" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="D60" t="s">
+        <v>11</v>
+      </c>
+      <c r="E60" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A61" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B61" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="C61" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="D61" t="s">
+        <v>11</v>
+      </c>
+      <c r="E61" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B62" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="C62" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="D62" t="s">
+        <v>11</v>
+      </c>
+      <c r="E62" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="B63" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C63" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="D63" t="s">
+        <v>11</v>
+      </c>
+      <c r="E63" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B64" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C64" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="D64" t="s">
+        <v>11</v>
+      </c>
+      <c r="E64" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A65" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="B65" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="C65" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="D65" t="s">
+        <v>11</v>
+      </c>
+      <c r="E65" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B66" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="C66" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="D66" t="s">
+        <v>93</v>
+      </c>
+      <c r="E66" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B67" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C67" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="D67" t="s">
+        <v>11</v>
+      </c>
+      <c r="E67" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B68" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C68" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="D68" t="s">
+        <v>11</v>
+      </c>
+      <c r="E68" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B69" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="C69" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="D69" t="s">
+        <v>11</v>
+      </c>
+      <c r="E69" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A70" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B70" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C70" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="D70" t="s">
+        <v>110</v>
+      </c>
+      <c r="E70" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B71" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="C71" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="D71" t="s">
+        <v>111</v>
+      </c>
+      <c r="E71" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A72" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B72" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="C72" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="D72" t="s">
+        <v>110</v>
+      </c>
+      <c r="E72" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="B73" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C73" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="D73" t="s">
+        <v>110</v>
+      </c>
+      <c r="E73" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A74" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B74" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="C74" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="D74" t="s">
+        <v>110</v>
+      </c>
+      <c r="E74" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A75" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="B75" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C75" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="D75" t="s">
+        <v>110</v>
+      </c>
+      <c r="E75" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A76" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="B76" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="C76" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="D76" t="s">
+        <v>111</v>
+      </c>
+      <c r="E76" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A77" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="B77" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="C77" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="D77" t="s">
+        <v>93</v>
+      </c>
+      <c r="E77" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A78" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="B78" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="C78" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="D78" t="s">
+        <v>111</v>
+      </c>
+      <c r="E78" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="B79" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="C79" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="D79" t="s">
+        <v>111</v>
+      </c>
+      <c r="E79" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A2:E2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F481C3AF-323B-446D-9A35-D97D9E1F1C4B}">
+  <dimension ref="A1:G4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.140625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="72.28515625" style="9" customWidth="1"/>
+    <col min="3" max="3" width="59.140625" style="9" customWidth="1"/>
+    <col min="4" max="4" width="26.140625" style="9" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>445</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
+        <v>446</v>
+      </c>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+    </row>
+    <row r="3" spans="1:7" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" s="5" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>448</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>447</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>221</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>425</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A2:E2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30B4B5ED-6412-48B2-94ED-1EEF687C55DD}">
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A1:XFD1048576"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2864,13 +4442,215 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA06AD4A-3D63-4FF3-B372-DF0ECFE24FED}">
+  <dimension ref="A1:G11"/>
+  <sheetViews>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="72.28515625" style="9" customWidth="1"/>
+    <col min="3" max="3" width="59.140625" style="9" customWidth="1"/>
+    <col min="4" max="4" width="26.140625" style="9" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>403</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
+        <v>404</v>
+      </c>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+    </row>
+    <row r="3" spans="1:7" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" s="5" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>405</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>413</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>221</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>425</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>406</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>427</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>426</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>435</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>407</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>428</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>429</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>436</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>408</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>430</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>431</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>437</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>409</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>442</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>443</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>438</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>410</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>444</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>432</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>439</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>411</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>433</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>434</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>412</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>440</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>441</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>438</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A2:E2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D8478C5-1713-4B9E-8DAE-5F54C2737D56}">
   <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B25" sqref="B25"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3339,7 +5119,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AD803A9-AF18-4300-9C9D-F24D7CF02CCF}">
   <dimension ref="A1:G7"/>
   <sheetViews>
@@ -3474,13 +5254,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5083188-FC9C-4563-81AC-AF6CFA6582AC}">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
+      <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3532,18 +5312,18 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="5" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" s="5" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>398</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>375</v>
+        <v>414</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>221</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>376</v>
+        <v>415</v>
       </c>
       <c r="E4" s="7" t="s">
         <v>9</v>
@@ -3554,7 +5334,7 @@
         <v>399</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>377</v>
+        <v>416</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>303</v>
@@ -3566,49 +5346,55 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>400</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>417</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>418</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>423</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>401</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="9" t="s">
+        <v>419</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>420</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>275</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>402</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
-        <v>408</v>
+      <c r="B8" s="9" t="s">
+        <v>421</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>422</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>424</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -3620,12 +5406,95 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C1F7F4E-C85C-485F-9096-69CB6FCB44F8}">
+  <dimension ref="A1:G4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="72.28515625" style="9" customWidth="1"/>
+    <col min="3" max="3" width="59.140625" style="9" customWidth="1"/>
+    <col min="4" max="4" width="26.140625" style="9" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>449</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
+        <v>450</v>
+      </c>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+    </row>
+    <row r="3" spans="1:7" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" s="5" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>451</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>452</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>221</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>453</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A2:E2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D14F67A4-A4C6-4846-971E-9E85D1BD727D}">
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="3" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -3805,1361 +5674,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65935663-0434-49C2-B8D3-B1FF868B4552}">
-  <dimension ref="A1:G79"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="10.140625" customWidth="1"/>
-    <col min="2" max="2" width="72.28515625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="50.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-    </row>
-    <row r="3" spans="1:7" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" t="s">
-        <v>11</v>
-      </c>
-      <c r="E10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E11" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" t="s">
-        <v>11</v>
-      </c>
-      <c r="E12" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D13" t="s">
-        <v>11</v>
-      </c>
-      <c r="E13" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D14" t="s">
-        <v>11</v>
-      </c>
-      <c r="E14" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D15" t="s">
-        <v>11</v>
-      </c>
-      <c r="E15" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D16" t="s">
-        <v>11</v>
-      </c>
-      <c r="E16" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D17" t="s">
-        <v>11</v>
-      </c>
-      <c r="E17" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D18" t="s">
-        <v>11</v>
-      </c>
-      <c r="E18" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D19" t="s">
-        <v>11</v>
-      </c>
-      <c r="E19" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D20" t="s">
-        <v>11</v>
-      </c>
-      <c r="E20" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D21" t="s">
-        <v>11</v>
-      </c>
-      <c r="E21" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D22" t="s">
-        <v>11</v>
-      </c>
-      <c r="E22" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D23" t="s">
-        <v>11</v>
-      </c>
-      <c r="E23" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D24" t="s">
-        <v>11</v>
-      </c>
-      <c r="E24" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D25" t="s">
-        <v>11</v>
-      </c>
-      <c r="E25" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D26" t="s">
-        <v>11</v>
-      </c>
-      <c r="E26" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D27" t="s">
-        <v>11</v>
-      </c>
-      <c r="E27" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D28" t="s">
-        <v>11</v>
-      </c>
-      <c r="E28" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D29" t="s">
-        <v>11</v>
-      </c>
-      <c r="E29" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D30" t="s">
-        <v>11</v>
-      </c>
-      <c r="E30" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D31" t="s">
-        <v>11</v>
-      </c>
-      <c r="E31" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D32" t="s">
-        <v>11</v>
-      </c>
-      <c r="E32" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D33" t="s">
-        <v>11</v>
-      </c>
-      <c r="E33" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D34" t="s">
-        <v>11</v>
-      </c>
-      <c r="E34" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D35" t="s">
-        <v>11</v>
-      </c>
-      <c r="E35" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="B36" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D36" t="s">
-        <v>11</v>
-      </c>
-      <c r="E36" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D37" t="s">
-        <v>11</v>
-      </c>
-      <c r="E37" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B38" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D38" t="s">
-        <v>11</v>
-      </c>
-      <c r="E38" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="B39" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C39" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D39" t="s">
-        <v>11</v>
-      </c>
-      <c r="E39" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="B40" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D40" t="s">
-        <v>11</v>
-      </c>
-      <c r="E40" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A41" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="B41" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="C41" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D41" t="s">
-        <v>11</v>
-      </c>
-      <c r="E41" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A42" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B42" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="C42" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D42" t="s">
-        <v>11</v>
-      </c>
-      <c r="E42" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A43" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B43" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="C43" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D43" t="s">
-        <v>11</v>
-      </c>
-      <c r="E43" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A44" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="B44" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C44" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D44" t="s">
-        <v>11</v>
-      </c>
-      <c r="E44" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A45" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="B45" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="C45" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D45" t="s">
-        <v>11</v>
-      </c>
-      <c r="E45" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A46" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="B46" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="C46" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D46" t="s">
-        <v>11</v>
-      </c>
-      <c r="E46" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A47" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="B47" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="C47" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D47" t="s">
-        <v>11</v>
-      </c>
-      <c r="E47" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A48" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="B48" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="C48" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D48" t="s">
-        <v>11</v>
-      </c>
-      <c r="E48" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="B49" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="C49" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="D49" t="s">
-        <v>93</v>
-      </c>
-      <c r="E49" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B50" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="C50" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="D50" t="s">
-        <v>93</v>
-      </c>
-      <c r="E50" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A51" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="B51" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="C51" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="D51" t="s">
-        <v>93</v>
-      </c>
-      <c r="E51" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A52" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="B52" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="C52" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="D52" t="s">
-        <v>11</v>
-      </c>
-      <c r="E52" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A53" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="B53" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="C53" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="D53" t="s">
-        <v>93</v>
-      </c>
-      <c r="E53" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A54" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="B54" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="C54" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="D54" t="s">
-        <v>93</v>
-      </c>
-      <c r="E54" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="B55" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="C55" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="D55" t="s">
-        <v>93</v>
-      </c>
-      <c r="E55" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="B56" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="C56" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="D56" t="s">
-        <v>11</v>
-      </c>
-      <c r="E56" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="B57" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="C57" s="4" t="s">
-        <v>164</v>
-      </c>
-      <c r="D57" t="s">
-        <v>11</v>
-      </c>
-      <c r="E57" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="B58" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="C58" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="D58" t="s">
-        <v>93</v>
-      </c>
-      <c r="E58" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A59" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="B59" s="4" t="s">
-        <v>190</v>
-      </c>
-      <c r="C59" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="D59" t="s">
-        <v>93</v>
-      </c>
-      <c r="E59" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B60" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="C60" s="4" t="s">
-        <v>186</v>
-      </c>
-      <c r="D60" t="s">
-        <v>11</v>
-      </c>
-      <c r="E60" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A61" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="B61" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="C61" s="4" t="s">
-        <v>166</v>
-      </c>
-      <c r="D61" t="s">
-        <v>11</v>
-      </c>
-      <c r="E61" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="B62" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="C62" s="4" t="s">
-        <v>167</v>
-      </c>
-      <c r="D62" t="s">
-        <v>11</v>
-      </c>
-      <c r="E62" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A63" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="B63" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="C63" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="D63" t="s">
-        <v>11</v>
-      </c>
-      <c r="E63" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A64" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="B64" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="C64" s="4" t="s">
-        <v>169</v>
-      </c>
-      <c r="D64" t="s">
-        <v>11</v>
-      </c>
-      <c r="E64" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A65" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="B65" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="C65" s="4" t="s">
-        <v>171</v>
-      </c>
-      <c r="D65" t="s">
-        <v>11</v>
-      </c>
-      <c r="E65" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="B66" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="C66" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="D66" t="s">
-        <v>93</v>
-      </c>
-      <c r="E66" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="B67" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="C67" s="4" t="s">
-        <v>174</v>
-      </c>
-      <c r="D67" t="s">
-        <v>11</v>
-      </c>
-      <c r="E67" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="B68" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="C68" s="4" t="s">
-        <v>174</v>
-      </c>
-      <c r="D68" t="s">
-        <v>11</v>
-      </c>
-      <c r="E68" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A69" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="B69" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="C69" s="4" t="s">
-        <v>176</v>
-      </c>
-      <c r="D69" t="s">
-        <v>11</v>
-      </c>
-      <c r="E69" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A70" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="B70" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="C70" s="4" t="s">
-        <v>171</v>
-      </c>
-      <c r="D70" t="s">
-        <v>110</v>
-      </c>
-      <c r="E70" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A71" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="B71" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="C71" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="D71" t="s">
-        <v>111</v>
-      </c>
-      <c r="E71" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A72" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="B72" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="C72" s="4" t="s">
-        <v>171</v>
-      </c>
-      <c r="D72" t="s">
-        <v>110</v>
-      </c>
-      <c r="E72" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A73" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="B73" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="C73" s="4" t="s">
-        <v>179</v>
-      </c>
-      <c r="D73" t="s">
-        <v>110</v>
-      </c>
-      <c r="E73" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A74" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="B74" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="C74" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="D74" t="s">
-        <v>110</v>
-      </c>
-      <c r="E74" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A75" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="B75" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="C75" s="4" t="s">
-        <v>181</v>
-      </c>
-      <c r="D75" t="s">
-        <v>110</v>
-      </c>
-      <c r="E75" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A76" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="B76" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="C76" s="4" t="s">
-        <v>182</v>
-      </c>
-      <c r="D76" t="s">
-        <v>111</v>
-      </c>
-      <c r="E76" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A77" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="B77" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="C77" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="D77" t="s">
-        <v>93</v>
-      </c>
-      <c r="E77" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A78" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="B78" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="C78" s="4" t="s">
-        <v>183</v>
-      </c>
-      <c r="D78" t="s">
-        <v>111</v>
-      </c>
-      <c r="E78" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A79" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="B79" s="4" t="s">
-        <v>187</v>
-      </c>
-      <c r="C79" s="4" t="s">
-        <v>182</v>
-      </c>
-      <c r="D79" t="s">
-        <v>111</v>
-      </c>
-      <c r="E79" t="s">
-        <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A2:E2"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Added Ground Design Requirements
</commit_message>
<xml_diff>
--- a/CougSat1/CougSat1-Requirements.xlsx
+++ b/CougSat1/CougSat1-Requirements.xlsx
@@ -8,20 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bradley\Documents\CougsInSpace\CougSat1-Hardware\CougSat1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E50B209-04E3-47D3-A10C-F48CFB72A75F}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2266E81-B1CF-4B6A-BE9A-735FD4670014}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="1" r:id="rId1"/>
     <sheet name="ADCS" sheetId="9" r:id="rId2"/>
     <sheet name="C&amp;DH" sheetId="6" r:id="rId3"/>
     <sheet name="Comms" sheetId="8" r:id="rId4"/>
-    <sheet name="EPS" sheetId="3" r:id="rId5"/>
-    <sheet name="ECS" sheetId="4" r:id="rId6"/>
-    <sheet name="IFJR" sheetId="7" r:id="rId7"/>
-    <sheet name="Payload" sheetId="10" r:id="rId8"/>
-    <sheet name="Structure" sheetId="5" r:id="rId9"/>
+    <sheet name="ECS" sheetId="4" r:id="rId5"/>
+    <sheet name="EPS" sheetId="3" r:id="rId6"/>
+    <sheet name="Ground" sheetId="11" r:id="rId7"/>
+    <sheet name="IFJR" sheetId="7" r:id="rId8"/>
+    <sheet name="Payload" sheetId="10" r:id="rId9"/>
+    <sheet name="Structure" sheetId="5" r:id="rId10"/>
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="374">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="400">
   <si>
     <t>CougSat-1 System Requirements</t>
   </si>
@@ -1155,6 +1156,84 @@
   </si>
   <si>
     <t>PAYLOAD-010</t>
+  </si>
+  <si>
+    <t>Ground Design Requirements</t>
+  </si>
+  <si>
+    <t>This sheet lists all of the design requirements of the Cougs in Space Ground Station</t>
+  </si>
+  <si>
+    <t>GND-000</t>
+  </si>
+  <si>
+    <t>GND-001</t>
+  </si>
+  <si>
+    <t>GND-002</t>
+  </si>
+  <si>
+    <t>GND-003</t>
+  </si>
+  <si>
+    <t>REQ-008, REQ-009, REQ-011, REQ-014, REQ-015, REQ-016, REQ-018, REQ-019, REQ-020, REQ-021, REQ-026, REQ-027, REQ-028, REQ-029</t>
+  </si>
+  <si>
+    <t>The Ground shall comply with all requirements listed below and all applicable system requirements</t>
+  </si>
+  <si>
+    <t>The Ground shall receive all forms of transmission from the Comms</t>
+  </si>
+  <si>
+    <t>The Ground shall transmit commands up to the Comms</t>
+  </si>
+  <si>
+    <t>The Ground shall be capable of autonomous reception for up to 10 days</t>
+  </si>
+  <si>
+    <t>The Ground may use cross-platform software</t>
+  </si>
+  <si>
+    <t>The Ground may have a website with the latest telemtry</t>
+  </si>
+  <si>
+    <t>The Ground shall have a RX only and a TX/RX version</t>
+  </si>
+  <si>
+    <t>GND-004</t>
+  </si>
+  <si>
+    <t>GND-005</t>
+  </si>
+  <si>
+    <t>GND-006</t>
+  </si>
+  <si>
+    <t>GND-007</t>
+  </si>
+  <si>
+    <t>The Ground is the other side of the communication system</t>
+  </si>
+  <si>
+    <t>Having the Ground with an operator for every pass is too much time and effort</t>
+  </si>
+  <si>
+    <t>Minimum is it must operate on Windows 10</t>
+  </si>
+  <si>
+    <t>The Ground shall transmit received data to a common repository</t>
+  </si>
+  <si>
+    <t>This archive will have all of the data of all of the satellites</t>
+  </si>
+  <si>
+    <t>Websites are an easy way to show the current status of the satellite to the general public</t>
+  </si>
+  <si>
+    <t>Only ground stations authorized by Cougs in Space will have TX capabilities for security</t>
+  </si>
+  <si>
+    <t>REQ-019, REQ-027</t>
   </si>
 </sst>
 </file>
@@ -1546,8 +1625,8 @@
   <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E3" sqref="E1:E1048576"/>
+      <pane ySplit="3" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2034,6 +2113,166 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D14F67A4-A4C6-4846-971E-9E85D1BD727D}">
+  <dimension ref="A1:F10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E3" sqref="E1:E1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="72.28515625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="59.140625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="26.140625" style="5" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+    </row>
+    <row r="3" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" s="1" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>200</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:D2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2680,11 +2919,128 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AD803A9-AF18-4300-9C9D-F24D7CF02CCF}">
+  <dimension ref="A1:F7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.140625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="72.28515625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="59.140625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="26.140625" style="5" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+    </row>
+    <row r="3" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" s="1" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:D2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D8478C5-1713-4B9E-8DAE-5F54C2737D56}">
   <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B22" sqref="B22:D23"/>
     </sheetView>
   </sheetViews>
@@ -3076,13 +3432,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AD803A9-AF18-4300-9C9D-F24D7CF02CCF}">
-  <dimension ref="A1:F7"/>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C23EDEE0-2306-4C9A-A2ED-349C7267C370}">
+  <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3096,7 +3451,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>163</v>
+        <v>374</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -3106,7 +3461,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>164</v>
+        <v>375</v>
       </c>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
@@ -3130,58 +3485,114 @@
     </row>
     <row r="4" spans="1:6" s="1" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>202</v>
+        <v>376</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>203</v>
+        <v>381</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>67</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>204</v>
+        <v>380</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>165</v>
+        <v>377</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>171</v>
+        <v>382</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>170</v>
+        <v>392</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>166</v>
+        <v>378</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>172</v>
+        <v>383</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>170</v>
+        <v>392</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>167</v>
+        <v>379</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>173</v>
+        <v>384</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>174</v>
+        <v>393</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>14</v>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>388</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>385</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>394</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>389</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>395</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>396</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>390</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>386</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>397</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>391</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>387</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>398</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -3193,7 +3604,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5083188-FC9C-4563-81AC-AF6CFA6582AC}">
   <dimension ref="A1:F10"/>
   <sheetViews>
@@ -3352,7 +3763,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C1F7F4E-C85C-485F-9096-69CB6FCB44F8}">
   <dimension ref="A1:F14"/>
   <sheetViews>
@@ -3564,164 +3975,4 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D14F67A4-A4C6-4846-971E-9E85D1BD727D}">
-  <dimension ref="A1:F10"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E3" sqref="E1:E1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="72.28515625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="59.140625" style="5" customWidth="1"/>
-    <col min="4" max="4" width="26.140625" style="5" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="3"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
-        <v>176</v>
-      </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-    </row>
-    <row r="3" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" s="1" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>192</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>186</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>188</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>189</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>190</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>231</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>194</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>199</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>201</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>200</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:D2"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>